<commit_message>
versie 1.0 SobekGraph en sobekgraph_tutorial gereed.
</commit_message>
<xml_diff>
--- a/tests/testdata/test.xlsx
+++ b/tests/testdata/test.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
     <sheet name="tijdstap3uur" sheetId="2" r:id="rId2"/>
     <sheet name="long time series" sheetId="3" r:id="rId3"/>
+    <sheet name="scope is 10" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>datum</t>
   </si>
@@ -876,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4784"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1068" workbookViewId="0">
-      <selection activeCell="C1100" sqref="C1100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C314" sqref="A1:C314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13418,7 +13419,7 @@
         <v>41222</v>
       </c>
       <c r="B1045">
-        <f t="shared" ref="B1045:B1108" si="17">SIN(PI()*C1045/144)</f>
+        <f t="shared" ref="B1045:B1097" si="17">SIN(PI()*C1045/144)</f>
         <v>-0.69151305578226718</v>
       </c>
       <c r="C1045">
@@ -25118,6 +25119,3791 @@
     </row>
     <row r="4784" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4784" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C314"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>40179</v>
+      </c>
+      <c r="B2">
+        <f>SIN(PI()*C2/144)*5</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>40180</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">SIN(PI()*C3/144)*5</f>
+        <v>0.10907442517280561</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>40181</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.21809693682667999</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>40182</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.32701564615071532</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>40183</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.4357787137382908</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>40184</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.5443343742598229</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>40185</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0.65263096110025787</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>40186</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.76061693094958349</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>40187</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.86824088833465163</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>40188</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.97545161008064118</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>40189</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1.0821980696905145</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>40190</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1.1884294616308653</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>40191</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1.2940952255126037</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>40192</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1.3991450701549604</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>40193</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1.5035289975213657</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>40194</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1.6071973265158077</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>40195</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>1.7101007166283435</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>40196</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>1.8121901914185081</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>40197</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>1.913417161825449</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>40198</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>2.013733449293686</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>40199</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>2.1130913087034973</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>40200</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>2.2114434510950067</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>40201</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>2.3087430661751691</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>40202</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>2.404943844596938</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>40203</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>2.4999999999999996</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>40204</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>2.5938662908026071</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>40205</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>2.6864980417341195</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>40206</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>2.7778511650980109</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>40207</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>2.8678821817552302</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>40208</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>2.9565482418179116</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>40209</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>3.0438071450436026</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>40210</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>3.1296173609202955</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>40211</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>3.2139380484326963</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>40212</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>3.2967290755003447</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>40213</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>3.3779510380783013</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>40214</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>3.4575652789113471</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>40215</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>3.5355339059327373</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>40216</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>3.6118198102987775</v>
+      </c>
+      <c r="C39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>40217</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>3.6863866840506199</v>
+      </c>
+      <c r="C40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>40218</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>3.7591990373948865</v>
+      </c>
+      <c r="C41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>40219</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>3.83022221559489</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>40220</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>3.8994224154644086</v>
+      </c>
+      <c r="C43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>40221</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>3.9667667014561756</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>40222</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>4.0322230213374128</v>
+      </c>
+      <c r="C45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>40223</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>4.0957602214449587</v>
+      </c>
+      <c r="C46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>40224</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>4.1573480615127263</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>40225</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>4.2169572290644286</v>
+      </c>
+      <c r="C48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>40226</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>4.2745593533647339</v>
+      </c>
+      <c r="C49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>40227</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>4.3301270189221928</v>
+      </c>
+      <c r="C50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>40228</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>4.3836337785375381</v>
+      </c>
+      <c r="C51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>40229</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>4.4350541658911089</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>40230</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>4.4843637076634417</v>
+      </c>
+      <c r="C53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>40231</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>4.5315389351832494</v>
+      </c>
+      <c r="C54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>40232</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>4.5765573955972352</v>
+      </c>
+      <c r="C55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>40233</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>4.6193976625564339</v>
+      </c>
+      <c r="C56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>40234</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>4.660039346413992</v>
+      </c>
+      <c r="C57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>40235</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>4.6984631039295417</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>40236</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>4.7346506474755277</v>
+      </c>
+      <c r="C59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>40237</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>4.768584753741135</v>
+      </c>
+      <c r="C60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>40238</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>4.8002492719296432</v>
+      </c>
+      <c r="C61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>40239</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>4.8296291314453406</v>
+      </c>
+      <c r="C62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>40240</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>4.8567103490663071</v>
+      </c>
+      <c r="C63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>40241</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>4.881480035599667</v>
+      </c>
+      <c r="C64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>40242</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>4.9039264020161522</v>
+      </c>
+      <c r="C65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>40243</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>4.9240387650610398</v>
+      </c>
+      <c r="C66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>40244</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B130" si="1">SIN(PI()*C67/144)*5</f>
+        <v>4.941807552338803</v>
+      </c>
+      <c r="C67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>40245</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>4.957224306869052</v>
+      </c>
+      <c r="C68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>40246</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>4.9702816911115981</v>
+      </c>
+      <c r="C69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>40247</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>4.9809734904587275</v>
+      </c>
+      <c r="C70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>40248</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>4.9892946161930176</v>
+      </c>
+      <c r="C71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>40249</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>4.9952411079092887</v>
+      </c>
+      <c r="C72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>40250</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>4.9988101353995456</v>
+      </c>
+      <c r="C73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>40251</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>40252</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>4.9988101353995456</v>
+      </c>
+      <c r="C75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>40253</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>4.9952411079092887</v>
+      </c>
+      <c r="C76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>40254</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>4.9892946161930176</v>
+      </c>
+      <c r="C77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>40255</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>4.9809734904587275</v>
+      </c>
+      <c r="C78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>40256</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>4.9702816911115981</v>
+      </c>
+      <c r="C79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>40257</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>4.9572243068690529</v>
+      </c>
+      <c r="C80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>40258</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>4.941807552338803</v>
+      </c>
+      <c r="C81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>40259</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="1"/>
+        <v>4.9240387650610398</v>
+      </c>
+      <c r="C82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>40260</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>4.9039264020161522</v>
+      </c>
+      <c r="C83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>40261</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>4.881480035599667</v>
+      </c>
+      <c r="C84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>40262</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>4.8567103490663071</v>
+      </c>
+      <c r="C85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>40263</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>4.8296291314453415</v>
+      </c>
+      <c r="C86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>40264</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>4.8002492719296432</v>
+      </c>
+      <c r="C87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>40265</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>4.768584753741135</v>
+      </c>
+      <c r="C88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>40266</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>4.7346506474755286</v>
+      </c>
+      <c r="C89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>40267</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>4.6984631039295426</v>
+      </c>
+      <c r="C90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>40268</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>4.6600393464139929</v>
+      </c>
+      <c r="C91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>40269</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>4.6193976625564339</v>
+      </c>
+      <c r="C92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>40270</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="1"/>
+        <v>4.5765573955972361</v>
+      </c>
+      <c r="C93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>40271</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="1"/>
+        <v>4.5315389351832502</v>
+      </c>
+      <c r="C94">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>40272</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="1"/>
+        <v>4.4843637076634417</v>
+      </c>
+      <c r="C95">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="1">
+        <v>40273</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="1"/>
+        <v>4.435054165891108</v>
+      </c>
+      <c r="C96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>40274</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="1"/>
+        <v>4.383633778537539</v>
+      </c>
+      <c r="C97">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
+        <v>40275</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="1"/>
+        <v>4.3301270189221936</v>
+      </c>
+      <c r="C98">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1">
+        <v>40276</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="1"/>
+        <v>4.2745593533647339</v>
+      </c>
+      <c r="C99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="1">
+        <v>40277</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="1"/>
+        <v>4.2169572290644295</v>
+      </c>
+      <c r="C100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>40278</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="1"/>
+        <v>4.1573480615127254</v>
+      </c>
+      <c r="C101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>40279</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="1"/>
+        <v>4.0957602214449587</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>40280</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="1"/>
+        <v>4.0322230213374128</v>
+      </c>
+      <c r="C103">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>40281</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="1"/>
+        <v>3.9667667014561756</v>
+      </c>
+      <c r="C104">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>40282</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="1"/>
+        <v>3.8994224154644104</v>
+      </c>
+      <c r="C105">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="1">
+        <v>40283</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="1"/>
+        <v>3.83022221559489</v>
+      </c>
+      <c r="C106">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>40284</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="1"/>
+        <v>3.7591990373948869</v>
+      </c>
+      <c r="C107">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>40285</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="1"/>
+        <v>3.6863866840506203</v>
+      </c>
+      <c r="C108">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>40286</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="1"/>
+        <v>3.611819810298778</v>
+      </c>
+      <c r="C109">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>40287</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="1"/>
+        <v>3.5355339059327378</v>
+      </c>
+      <c r="C110">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" s="1">
+        <v>40288</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="1"/>
+        <v>3.4575652789113476</v>
+      </c>
+      <c r="C111">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>40289</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="1"/>
+        <v>3.3779510380783018</v>
+      </c>
+      <c r="C112">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
+        <v>40290</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="1"/>
+        <v>3.2967290755003447</v>
+      </c>
+      <c r="C113">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
+        <v>40291</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="1"/>
+        <v>3.2139380484326976</v>
+      </c>
+      <c r="C114">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>40292</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="1"/>
+        <v>3.129617360920296</v>
+      </c>
+      <c r="C115">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>40293</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="1"/>
+        <v>3.0438071450436044</v>
+      </c>
+      <c r="C116">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="1">
+        <v>40294</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="1"/>
+        <v>2.9565482418179112</v>
+      </c>
+      <c r="C117">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>40295</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="1"/>
+        <v>2.8678821817552298</v>
+      </c>
+      <c r="C118">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>40296</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="1"/>
+        <v>2.7778511650980109</v>
+      </c>
+      <c r="C119">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="1">
+        <v>40297</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="1"/>
+        <v>2.6864980417341204</v>
+      </c>
+      <c r="C120">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>40298</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="1"/>
+        <v>2.5938662908026089</v>
+      </c>
+      <c r="C121">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="1">
+        <v>40299</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000018</v>
+      </c>
+      <c r="C122">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>40300</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="1"/>
+        <v>2.404943844596938</v>
+      </c>
+      <c r="C123">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>40301</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="1"/>
+        <v>2.3087430661751696</v>
+      </c>
+      <c r="C124">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="1">
+        <v>40302</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="1"/>
+        <v>2.2114434510950067</v>
+      </c>
+      <c r="C125">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" s="1">
+        <v>40303</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="1"/>
+        <v>2.1130913087034973</v>
+      </c>
+      <c r="C126">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>40304</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="1"/>
+        <v>2.0137334492936865</v>
+      </c>
+      <c r="C127">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="1">
+        <v>40305</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="1"/>
+        <v>1.9134171618254494</v>
+      </c>
+      <c r="C128">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>40306</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="1"/>
+        <v>1.8121901914185088</v>
+      </c>
+      <c r="C129">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="1">
+        <v>40307</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="1"/>
+        <v>1.7101007166283444</v>
+      </c>
+      <c r="C130">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="1">
+        <v>40308</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:B194" si="2">SIN(PI()*C131/144)*5</f>
+        <v>1.6071973265158088</v>
+      </c>
+      <c r="C131">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="1">
+        <v>40309</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="2"/>
+        <v>1.5035289975213666</v>
+      </c>
+      <c r="C132">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="1">
+        <v>40310</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="2"/>
+        <v>1.3991450701549593</v>
+      </c>
+      <c r="C133">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="1">
+        <v>40311</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="2"/>
+        <v>1.2940952255126028</v>
+      </c>
+      <c r="C134">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="1">
+        <v>40312</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="2"/>
+        <v>1.1884294616308668</v>
+      </c>
+      <c r="C135">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="1">
+        <v>40313</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="2"/>
+        <v>1.082198069690516</v>
+      </c>
+      <c r="C136">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="1">
+        <v>40314</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="2"/>
+        <v>0.97545161008064307</v>
+      </c>
+      <c r="C137">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="1">
+        <v>40315</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="2"/>
+        <v>0.86824088833465141</v>
+      </c>
+      <c r="C138">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="1">
+        <v>40316</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="2"/>
+        <v>0.76061693094958316</v>
+      </c>
+      <c r="C139">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="1">
+        <v>40317</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="2"/>
+        <v>0.65263096110025787</v>
+      </c>
+      <c r="C140">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="1">
+        <v>40318</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="2"/>
+        <v>0.5443343742598229</v>
+      </c>
+      <c r="C141">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="1">
+        <v>40319</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="2"/>
+        <v>0.43577871373829097</v>
+      </c>
+      <c r="C142">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="1">
+        <v>40320</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="2"/>
+        <v>0.32701564615071782</v>
+      </c>
+      <c r="C143">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="1">
+        <v>40321</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="2"/>
+        <v>0.21809693682668035</v>
+      </c>
+      <c r="C144">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="1">
+        <v>40322</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="2"/>
+        <v>0.10907442517280609</v>
+      </c>
+      <c r="C145">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="1">
+        <v>40323</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="2"/>
+        <v>6.1257422745431001E-16</v>
+      </c>
+      <c r="C146">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" s="1">
+        <v>40324</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="2"/>
+        <v>-0.10907442517280487</v>
+      </c>
+      <c r="C147">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="1">
+        <v>40325</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="2"/>
+        <v>-0.21809693682667913</v>
+      </c>
+      <c r="C148">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="1">
+        <v>40326</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="2"/>
+        <v>-0.32701564615071654</v>
+      </c>
+      <c r="C149">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="1">
+        <v>40327</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="2"/>
+        <v>-0.43577871373828969</v>
+      </c>
+      <c r="C150">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" s="1">
+        <v>40328</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="2"/>
+        <v>-0.54433437425982156</v>
+      </c>
+      <c r="C151">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" s="1">
+        <v>40329</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="2"/>
+        <v>-0.65263096110025665</v>
+      </c>
+      <c r="C152">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" s="1">
+        <v>40330</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="2"/>
+        <v>-0.76061693094958205</v>
+      </c>
+      <c r="C153">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="1">
+        <v>40331</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="2"/>
+        <v>-0.86824088833465018</v>
+      </c>
+      <c r="C154">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" s="1">
+        <v>40332</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="2"/>
+        <v>-0.97545161008064185</v>
+      </c>
+      <c r="C155">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" s="1">
+        <v>40333</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="2"/>
+        <v>-1.0821980696905147</v>
+      </c>
+      <c r="C156">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" s="1">
+        <v>40334</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="2"/>
+        <v>-1.1884294616308657</v>
+      </c>
+      <c r="C157">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" s="1">
+        <v>40335</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="2"/>
+        <v>-1.2940952255126017</v>
+      </c>
+      <c r="C158">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" s="1">
+        <v>40336</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="2"/>
+        <v>-1.3991450701549581</v>
+      </c>
+      <c r="C159">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" s="1">
+        <v>40337</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="2"/>
+        <v>-1.5035289975213653</v>
+      </c>
+      <c r="C160">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="1">
+        <v>40338</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="2"/>
+        <v>-1.6071973265158077</v>
+      </c>
+      <c r="C161">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" s="1">
+        <v>40339</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="2"/>
+        <v>-1.7101007166283433</v>
+      </c>
+      <c r="C162">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" s="1">
+        <v>40340</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="2"/>
+        <v>-1.8121901914185077</v>
+      </c>
+      <c r="C163">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="1">
+        <v>40341</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="2"/>
+        <v>-1.9134171618254483</v>
+      </c>
+      <c r="C164">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" s="1">
+        <v>40342</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="2"/>
+        <v>-2.0137334492936851</v>
+      </c>
+      <c r="C165">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" s="1">
+        <v>40343</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="2"/>
+        <v>-2.1130913087034946</v>
+      </c>
+      <c r="C166">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" s="1">
+        <v>40344</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="2"/>
+        <v>-2.2114434510950036</v>
+      </c>
+      <c r="C167">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" s="1">
+        <v>40345</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="2"/>
+        <v>-2.3087430661751709</v>
+      </c>
+      <c r="C168">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="1">
+        <v>40346</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="2"/>
+        <v>-2.4049438445969389</v>
+      </c>
+      <c r="C169">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="1">
+        <v>40347</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="2"/>
+        <v>-2.5000000000000004</v>
+      </c>
+      <c r="C170">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="1">
+        <v>40348</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="2"/>
+        <v>-2.593866290802608</v>
+      </c>
+      <c r="C171">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="1">
+        <v>40349</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="2"/>
+        <v>-2.6864980417341195</v>
+      </c>
+      <c r="C172">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="1">
+        <v>40350</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="2"/>
+        <v>-2.77785116509801</v>
+      </c>
+      <c r="C173">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="1">
+        <v>40351</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="2"/>
+        <v>-2.8678821817552294</v>
+      </c>
+      <c r="C174">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" s="1">
+        <v>40352</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="2"/>
+        <v>-2.9565482418179103</v>
+      </c>
+      <c r="C175">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="1">
+        <v>40353</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="2"/>
+        <v>-3.0438071450436017</v>
+      </c>
+      <c r="C176">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" s="1">
+        <v>40354</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="2"/>
+        <v>-3.1296173609202937</v>
+      </c>
+      <c r="C177">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" s="1">
+        <v>40355</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="2"/>
+        <v>-3.2139380484326945</v>
+      </c>
+      <c r="C178">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" s="1">
+        <v>40356</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="2"/>
+        <v>-3.296729075500346</v>
+      </c>
+      <c r="C179">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" s="1">
+        <v>40357</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="2"/>
+        <v>-3.3779510380783009</v>
+      </c>
+      <c r="C180">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" s="1">
+        <v>40358</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="2"/>
+        <v>-3.4575652789113462</v>
+      </c>
+      <c r="C181">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" s="1">
+        <v>40359</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="2"/>
+        <v>-3.5355339059327373</v>
+      </c>
+      <c r="C182">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" s="1">
+        <v>40360</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="2"/>
+        <v>-3.6118198102987775</v>
+      </c>
+      <c r="C183">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" s="1">
+        <v>40361</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="2"/>
+        <v>-3.6863866840506194</v>
+      </c>
+      <c r="C184">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" s="1">
+        <v>40362</v>
+      </c>
+      <c r="B185">
+        <f t="shared" si="2"/>
+        <v>-3.7591990373948865</v>
+      </c>
+      <c r="C185">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" s="1">
+        <v>40363</v>
+      </c>
+      <c r="B186">
+        <f t="shared" si="2"/>
+        <v>-3.8302222155948895</v>
+      </c>
+      <c r="C186">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" s="1">
+        <v>40364</v>
+      </c>
+      <c r="B187">
+        <f t="shared" si="2"/>
+        <v>-3.8994224154644068</v>
+      </c>
+      <c r="C187">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A188" s="1">
+        <v>40365</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="2"/>
+        <v>-3.9667667014561747</v>
+      </c>
+      <c r="C188">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" s="1">
+        <v>40366</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="2"/>
+        <v>-4.0322230213374137</v>
+      </c>
+      <c r="C189">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A190" s="1">
+        <v>40367</v>
+      </c>
+      <c r="B190">
+        <f t="shared" si="2"/>
+        <v>-4.0957602214449604</v>
+      </c>
+      <c r="C190">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" s="1">
+        <v>40368</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="2"/>
+        <v>-4.1573480615127263</v>
+      </c>
+      <c r="C191">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" s="1">
+        <v>40369</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="2"/>
+        <v>-4.2169572290644277</v>
+      </c>
+      <c r="C192">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" s="1">
+        <v>40370</v>
+      </c>
+      <c r="B193">
+        <f t="shared" si="2"/>
+        <v>-4.274559353364733</v>
+      </c>
+      <c r="C193">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" s="1">
+        <v>40371</v>
+      </c>
+      <c r="B194">
+        <f t="shared" si="2"/>
+        <v>-4.3301270189221919</v>
+      </c>
+      <c r="C194">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" s="1">
+        <v>40372</v>
+      </c>
+      <c r="B195">
+        <f t="shared" ref="B195:B258" si="3">SIN(PI()*C195/144)*5</f>
+        <v>-4.3836337785375381</v>
+      </c>
+      <c r="C195">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" s="1">
+        <v>40373</v>
+      </c>
+      <c r="B196">
+        <f t="shared" si="3"/>
+        <v>-4.4350541658911071</v>
+      </c>
+      <c r="C196">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" s="1">
+        <v>40374</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="3"/>
+        <v>-4.4843637076634408</v>
+      </c>
+      <c r="C197">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A198" s="1">
+        <v>40375</v>
+      </c>
+      <c r="B198">
+        <f t="shared" si="3"/>
+        <v>-4.5315389351832485</v>
+      </c>
+      <c r="C198">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A199" s="1">
+        <v>40376</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="3"/>
+        <v>-4.5765573955972352</v>
+      </c>
+      <c r="C199">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A200" s="1">
+        <v>40377</v>
+      </c>
+      <c r="B200">
+        <f t="shared" si="3"/>
+        <v>-4.6193976625564339</v>
+      </c>
+      <c r="C200">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A201" s="1">
+        <v>40378</v>
+      </c>
+      <c r="B201">
+        <f t="shared" si="3"/>
+        <v>-4.660039346413992</v>
+      </c>
+      <c r="C201">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A202" s="1">
+        <v>40379</v>
+      </c>
+      <c r="B202">
+        <f t="shared" si="3"/>
+        <v>-4.6984631039295426</v>
+      </c>
+      <c r="C202">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A203" s="1">
+        <v>40380</v>
+      </c>
+      <c r="B203">
+        <f t="shared" si="3"/>
+        <v>-4.7346506474755277</v>
+      </c>
+      <c r="C203">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A204" s="1">
+        <v>40381</v>
+      </c>
+      <c r="B204">
+        <f t="shared" si="3"/>
+        <v>-4.768584753741135</v>
+      </c>
+      <c r="C204">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A205" s="1">
+        <v>40382</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="3"/>
+        <v>-4.8002492719296432</v>
+      </c>
+      <c r="C205">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A206" s="1">
+        <v>40383</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="3"/>
+        <v>-4.8296291314453415</v>
+      </c>
+      <c r="C206">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A207" s="1">
+        <v>40384</v>
+      </c>
+      <c r="B207">
+        <f t="shared" si="3"/>
+        <v>-4.8567103490663062</v>
+      </c>
+      <c r="C207">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A208" s="1">
+        <v>40385</v>
+      </c>
+      <c r="B208">
+        <f t="shared" si="3"/>
+        <v>-4.8814800355996653</v>
+      </c>
+      <c r="C208">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A209" s="1">
+        <v>40386</v>
+      </c>
+      <c r="B209">
+        <f t="shared" si="3"/>
+        <v>-4.9039264020161513</v>
+      </c>
+      <c r="C209">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A210" s="1">
+        <v>40387</v>
+      </c>
+      <c r="B210">
+        <f t="shared" si="3"/>
+        <v>-4.9240387650610398</v>
+      </c>
+      <c r="C210">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A211" s="1">
+        <v>40388</v>
+      </c>
+      <c r="B211">
+        <f t="shared" si="3"/>
+        <v>-4.9418075523388039</v>
+      </c>
+      <c r="C211">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A212" s="1">
+        <v>40389</v>
+      </c>
+      <c r="B212">
+        <f t="shared" si="3"/>
+        <v>-4.957224306869052</v>
+      </c>
+      <c r="C212">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A213" s="1">
+        <v>40390</v>
+      </c>
+      <c r="B213">
+        <f t="shared" si="3"/>
+        <v>-4.9702816911115981</v>
+      </c>
+      <c r="C213">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A214" s="1">
+        <v>40391</v>
+      </c>
+      <c r="B214">
+        <f t="shared" si="3"/>
+        <v>-4.9809734904587275</v>
+      </c>
+      <c r="C214">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A215" s="1">
+        <v>40392</v>
+      </c>
+      <c r="B215">
+        <f t="shared" si="3"/>
+        <v>-4.9892946161930176</v>
+      </c>
+      <c r="C215">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A216" s="1">
+        <v>40393</v>
+      </c>
+      <c r="B216">
+        <f t="shared" si="3"/>
+        <v>-4.9952411079092887</v>
+      </c>
+      <c r="C216">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A217" s="1">
+        <v>40394</v>
+      </c>
+      <c r="B217">
+        <f t="shared" si="3"/>
+        <v>-4.9988101353995456</v>
+      </c>
+      <c r="C217">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A218" s="1">
+        <v>40395</v>
+      </c>
+      <c r="B218">
+        <f t="shared" si="3"/>
+        <v>-5</v>
+      </c>
+      <c r="C218">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A219" s="1">
+        <v>40396</v>
+      </c>
+      <c r="B219">
+        <f t="shared" si="3"/>
+        <v>-4.9988101353995456</v>
+      </c>
+      <c r="C219">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A220" s="1">
+        <v>40397</v>
+      </c>
+      <c r="B220">
+        <f t="shared" si="3"/>
+        <v>-4.9952411079092887</v>
+      </c>
+      <c r="C220">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" s="1">
+        <v>40398</v>
+      </c>
+      <c r="B221">
+        <f t="shared" si="3"/>
+        <v>-4.9892946161930176</v>
+      </c>
+      <c r="C221">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" s="1">
+        <v>40399</v>
+      </c>
+      <c r="B222">
+        <f t="shared" si="3"/>
+        <v>-4.9809734904587275</v>
+      </c>
+      <c r="C222">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" s="1">
+        <v>40400</v>
+      </c>
+      <c r="B223">
+        <f t="shared" si="3"/>
+        <v>-4.9702816911115981</v>
+      </c>
+      <c r="C223">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" s="1">
+        <v>40401</v>
+      </c>
+      <c r="B224">
+        <f t="shared" si="3"/>
+        <v>-4.9572243068690529</v>
+      </c>
+      <c r="C224">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" s="1">
+        <v>40402</v>
+      </c>
+      <c r="B225">
+        <f t="shared" si="3"/>
+        <v>-4.941807552338803</v>
+      </c>
+      <c r="C225">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" s="1">
+        <v>40403</v>
+      </c>
+      <c r="B226">
+        <f t="shared" si="3"/>
+        <v>-4.9240387650610407</v>
+      </c>
+      <c r="C226">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A227" s="1">
+        <v>40404</v>
+      </c>
+      <c r="B227">
+        <f t="shared" si="3"/>
+        <v>-4.9039264020161522</v>
+      </c>
+      <c r="C227">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" s="1">
+        <v>40405</v>
+      </c>
+      <c r="B228">
+        <f t="shared" si="3"/>
+        <v>-4.881480035599667</v>
+      </c>
+      <c r="C228">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" s="1">
+        <v>40406</v>
+      </c>
+      <c r="B229">
+        <f t="shared" si="3"/>
+        <v>-4.8567103490663071</v>
+      </c>
+      <c r="C229">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A230" s="1">
+        <v>40407</v>
+      </c>
+      <c r="B230">
+        <f t="shared" si="3"/>
+        <v>-4.8296291314453423</v>
+      </c>
+      <c r="C230">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A231" s="1">
+        <v>40408</v>
+      </c>
+      <c r="B231">
+        <f t="shared" si="3"/>
+        <v>-4.800249271929645</v>
+      </c>
+      <c r="C231">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A232" s="1">
+        <v>40409</v>
+      </c>
+      <c r="B232">
+        <f t="shared" si="3"/>
+        <v>-4.7685847537411341</v>
+      </c>
+      <c r="C232">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A233" s="1">
+        <v>40410</v>
+      </c>
+      <c r="B233">
+        <f t="shared" si="3"/>
+        <v>-4.7346506474755286</v>
+      </c>
+      <c r="C233">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A234" s="1">
+        <v>40411</v>
+      </c>
+      <c r="B234">
+        <f t="shared" si="3"/>
+        <v>-4.6984631039295417</v>
+      </c>
+      <c r="C234">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A235" s="1">
+        <v>40412</v>
+      </c>
+      <c r="B235">
+        <f t="shared" si="3"/>
+        <v>-4.6600393464139929</v>
+      </c>
+      <c r="C235">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A236" s="1">
+        <v>40413</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="3"/>
+        <v>-4.619397662556433</v>
+      </c>
+      <c r="C236">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A237" s="1">
+        <v>40414</v>
+      </c>
+      <c r="B237">
+        <f t="shared" si="3"/>
+        <v>-4.5765573955972361</v>
+      </c>
+      <c r="C237">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A238" s="1">
+        <v>40415</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="3"/>
+        <v>-4.5315389351832511</v>
+      </c>
+      <c r="C238">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A239" s="1">
+        <v>40416</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="3"/>
+        <v>-4.4843637076634426</v>
+      </c>
+      <c r="C239">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A240" s="1">
+        <v>40417</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="3"/>
+        <v>-4.4350541658911098</v>
+      </c>
+      <c r="C240">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A241" s="1">
+        <v>40418</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="3"/>
+        <v>-4.3836337785375399</v>
+      </c>
+      <c r="C241">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A242" s="1">
+        <v>40419</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="3"/>
+        <v>-4.3301270189221954</v>
+      </c>
+      <c r="C242">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A243" s="1">
+        <v>40420</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="3"/>
+        <v>-4.2745593533647321</v>
+      </c>
+      <c r="C243">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A244" s="1">
+        <v>40421</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="3"/>
+        <v>-4.2169572290644286</v>
+      </c>
+      <c r="C244">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A245" s="1">
+        <v>40422</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="3"/>
+        <v>-4.1573480615127272</v>
+      </c>
+      <c r="C245">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A246" s="1">
+        <v>40423</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="3"/>
+        <v>-4.0957602214449587</v>
+      </c>
+      <c r="C246">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A247" s="1">
+        <v>40424</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="3"/>
+        <v>-4.0322230213374146</v>
+      </c>
+      <c r="C247">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A248" s="1">
+        <v>40425</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="3"/>
+        <v>-3.9667667014561756</v>
+      </c>
+      <c r="C248">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A249" s="1">
+        <v>40426</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="3"/>
+        <v>-3.8994224154644108</v>
+      </c>
+      <c r="C249">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A250" s="1">
+        <v>40427</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="3"/>
+        <v>-3.8302222155948904</v>
+      </c>
+      <c r="C250">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A251" s="1">
+        <v>40428</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="3"/>
+        <v>-3.7591990373948891</v>
+      </c>
+      <c r="C251">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A252" s="1">
+        <v>40429</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="3"/>
+        <v>-3.6863866840506212</v>
+      </c>
+      <c r="C252">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A253" s="1">
+        <v>40430</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="3"/>
+        <v>-3.6118198102987771</v>
+      </c>
+      <c r="C253">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A254" s="1">
+        <v>40431</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="3"/>
+        <v>-3.5355339059327386</v>
+      </c>
+      <c r="C254">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A255" s="1">
+        <v>40432</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="3"/>
+        <v>-3.4575652789113458</v>
+      </c>
+      <c r="C255">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A256" s="1">
+        <v>40433</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="3"/>
+        <v>-3.3779510380783022</v>
+      </c>
+      <c r="C256">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A257" s="1">
+        <v>40434</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="3"/>
+        <v>-3.2967290755003438</v>
+      </c>
+      <c r="C257">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A258" s="1">
+        <v>40435</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="3"/>
+        <v>-3.213938048432698</v>
+      </c>
+      <c r="C258">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A259" s="1">
+        <v>40436</v>
+      </c>
+      <c r="B259">
+        <f t="shared" ref="B259:B314" si="4">SIN(PI()*C259/144)*5</f>
+        <v>-3.1296173609202951</v>
+      </c>
+      <c r="C259">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A260" s="1">
+        <v>40437</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="4"/>
+        <v>-3.0438071450436044</v>
+      </c>
+      <c r="C260">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A261" s="1">
+        <v>40438</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="4"/>
+        <v>-2.9565482418179152</v>
+      </c>
+      <c r="C261">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A262" s="1">
+        <v>40439</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="4"/>
+        <v>-2.8678821817552325</v>
+      </c>
+      <c r="C262">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A263" s="1">
+        <v>40440</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="4"/>
+        <v>-2.7778511650980149</v>
+      </c>
+      <c r="C263">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A264" s="1">
+        <v>40441</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="4"/>
+        <v>-2.6864980417341173</v>
+      </c>
+      <c r="C264">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A265" s="1">
+        <v>40442</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="4"/>
+        <v>-2.5938662908026071</v>
+      </c>
+      <c r="C265">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A266" s="1">
+        <v>40443</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="4"/>
+        <v>-2.4999999999999982</v>
+      </c>
+      <c r="C266">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A267" s="1">
+        <v>40444</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="4"/>
+        <v>-2.4049438445969389</v>
+      </c>
+      <c r="C267">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A268" s="1">
+        <v>40445</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="4"/>
+        <v>-2.3087430661751722</v>
+      </c>
+      <c r="C268">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A269" s="1">
+        <v>40446</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="4"/>
+        <v>-2.2114434510950072</v>
+      </c>
+      <c r="C269">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A270" s="1">
+        <v>40447</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="4"/>
+        <v>-2.1130913087034999</v>
+      </c>
+      <c r="C270">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A271" s="1">
+        <v>40448</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="4"/>
+        <v>-2.0137334492936869</v>
+      </c>
+      <c r="C271">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A272" s="1">
+        <v>40449</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="4"/>
+        <v>-1.9134171618254521</v>
+      </c>
+      <c r="C272">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A273" s="1">
+        <v>40450</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="4"/>
+        <v>-1.8121901914185092</v>
+      </c>
+      <c r="C273">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A274" s="1">
+        <v>40451</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="4"/>
+        <v>-1.7101007166283431</v>
+      </c>
+      <c r="C274">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A275" s="1">
+        <v>40452</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="4"/>
+        <v>-1.6071973265158093</v>
+      </c>
+      <c r="C275">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A276" s="1">
+        <v>40453</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="4"/>
+        <v>-1.503528997521365</v>
+      </c>
+      <c r="C276">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A277" s="1">
+        <v>40454</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="4"/>
+        <v>-1.3991450701549621</v>
+      </c>
+      <c r="C277">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A278" s="1">
+        <v>40455</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="4"/>
+        <v>-1.2940952255126035</v>
+      </c>
+      <c r="C278">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A279" s="1">
+        <v>40456</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="4"/>
+        <v>-1.1884294616308675</v>
+      </c>
+      <c r="C279">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A280" s="1">
+        <v>40457</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="4"/>
+        <v>-1.0821980696905145</v>
+      </c>
+      <c r="C280">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A281" s="1">
+        <v>40458</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="4"/>
+        <v>-0.97545161008064363</v>
+      </c>
+      <c r="C281">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A282" s="1">
+        <v>40459</v>
+      </c>
+      <c r="B282">
+        <f t="shared" si="4"/>
+        <v>-0.86824088833465196</v>
+      </c>
+      <c r="C282">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A283" s="1">
+        <v>40460</v>
+      </c>
+      <c r="B283">
+        <f t="shared" si="4"/>
+        <v>-0.76061693094958593</v>
+      </c>
+      <c r="C283">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A284" s="1">
+        <v>40461</v>
+      </c>
+      <c r="B284">
+        <f t="shared" si="4"/>
+        <v>-0.65263096110026286</v>
+      </c>
+      <c r="C284">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A285" s="1">
+        <v>40462</v>
+      </c>
+      <c r="B285">
+        <f t="shared" si="4"/>
+        <v>-0.54433437425982123</v>
+      </c>
+      <c r="C285">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A286" s="1">
+        <v>40463</v>
+      </c>
+      <c r="B286">
+        <f t="shared" si="4"/>
+        <v>-0.43577871373829158</v>
+      </c>
+      <c r="C286">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A287" s="1">
+        <v>40464</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="4"/>
+        <v>-0.32701564615071399</v>
+      </c>
+      <c r="C287">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A288" s="1">
+        <v>40465</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="4"/>
+        <v>-0.21809693682668096</v>
+      </c>
+      <c r="C288">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A289" s="1">
+        <v>40466</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="4"/>
+        <v>-0.1090744251728045</v>
+      </c>
+      <c r="C289">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A290" s="1">
+        <v>40467</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="4"/>
+        <v>-1.22514845490862E-15</v>
+      </c>
+      <c r="C290">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A291" s="1">
+        <v>40468</v>
+      </c>
+      <c r="B291">
+        <f t="shared" si="4"/>
+        <v>0.10907442517280203</v>
+      </c>
+      <c r="C291">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A292" s="1">
+        <v>40469</v>
+      </c>
+      <c r="B292">
+        <f t="shared" si="4"/>
+        <v>0.21809693682667852</v>
+      </c>
+      <c r="C292">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A293" s="1">
+        <v>40470</v>
+      </c>
+      <c r="B293">
+        <f t="shared" si="4"/>
+        <v>0.32701564615071149</v>
+      </c>
+      <c r="C293">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A294" s="1">
+        <v>40471</v>
+      </c>
+      <c r="B294">
+        <f t="shared" si="4"/>
+        <v>0.43577871373828914</v>
+      </c>
+      <c r="C294">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A295" s="1">
+        <v>40472</v>
+      </c>
+      <c r="B295">
+        <f t="shared" si="4"/>
+        <v>0.54433437425981879</v>
+      </c>
+      <c r="C295">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A296" s="1">
+        <v>40473</v>
+      </c>
+      <c r="B296">
+        <f t="shared" si="4"/>
+        <v>0.65263096110026031</v>
+      </c>
+      <c r="C296">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A297" s="1">
+        <v>40474</v>
+      </c>
+      <c r="B297">
+        <f t="shared" si="4"/>
+        <v>0.7606169309495836</v>
+      </c>
+      <c r="C297">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A298" s="1">
+        <v>40475</v>
+      </c>
+      <c r="B298">
+        <f t="shared" si="4"/>
+        <v>0.86824088833464952</v>
+      </c>
+      <c r="C298">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A299" s="1">
+        <v>40476</v>
+      </c>
+      <c r="B299">
+        <f t="shared" si="4"/>
+        <v>0.97545161008064118</v>
+      </c>
+      <c r="C299">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A300" s="1">
+        <v>40477</v>
+      </c>
+      <c r="B300">
+        <f t="shared" si="4"/>
+        <v>1.082198069690512</v>
+      </c>
+      <c r="C300">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A301" s="1">
+        <v>40478</v>
+      </c>
+      <c r="B301">
+        <f t="shared" si="4"/>
+        <v>1.188429461630865</v>
+      </c>
+      <c r="C301">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A302" s="1">
+        <v>40479</v>
+      </c>
+      <c r="B302">
+        <f t="shared" si="4"/>
+        <v>1.2940952255126013</v>
+      </c>
+      <c r="C302">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A303" s="1">
+        <v>40480</v>
+      </c>
+      <c r="B303">
+        <f t="shared" si="4"/>
+        <v>1.3991450701549595</v>
+      </c>
+      <c r="C303">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A304" s="1">
+        <v>40481</v>
+      </c>
+      <c r="B304">
+        <f t="shared" si="4"/>
+        <v>1.5035289975213628</v>
+      </c>
+      <c r="C304">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A305" s="1">
+        <v>40482</v>
+      </c>
+      <c r="B305">
+        <f t="shared" si="4"/>
+        <v>1.607197326515807</v>
+      </c>
+      <c r="C305">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A306" s="1">
+        <v>40483</v>
+      </c>
+      <c r="B306">
+        <f t="shared" si="4"/>
+        <v>1.7101007166283404</v>
+      </c>
+      <c r="C306">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A307" s="1">
+        <v>40484</v>
+      </c>
+      <c r="B307">
+        <f t="shared" si="4"/>
+        <v>1.812190191418507</v>
+      </c>
+      <c r="C307">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A308" s="1">
+        <v>40485</v>
+      </c>
+      <c r="B308">
+        <f t="shared" si="4"/>
+        <v>1.9134171618254499</v>
+      </c>
+      <c r="C308">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A309" s="1">
+        <v>40486</v>
+      </c>
+      <c r="B309">
+        <f t="shared" si="4"/>
+        <v>2.0137334492936847</v>
+      </c>
+      <c r="C309">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A310" s="1">
+        <v>40487</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="4"/>
+        <v>2.1130913087034977</v>
+      </c>
+      <c r="C310">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A311" s="1">
+        <v>40488</v>
+      </c>
+      <c r="B311">
+        <f t="shared" si="4"/>
+        <v>2.211443451095005</v>
+      </c>
+      <c r="C311">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A312" s="1">
+        <v>40489</v>
+      </c>
+      <c r="B312">
+        <f t="shared" si="4"/>
+        <v>2.30874306617517</v>
+      </c>
+      <c r="C312">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A313" s="1">
+        <v>40490</v>
+      </c>
+      <c r="B313">
+        <f t="shared" si="4"/>
+        <v>2.4049438445969367</v>
+      </c>
+      <c r="C313">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A314" s="1">
+        <v>40491</v>
+      </c>
+      <c r="B314">
+        <f t="shared" si="4"/>
+        <v>2.4999999999999964</v>
+      </c>
+      <c r="C314">
+        <v>312</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>